<commit_message>
project: fixed indexing in reg_obl_city from 1, not from 2
</commit_message>
<xml_diff>
--- a/data/Reg_obl_city.xlsx
+++ b/data/Reg_obl_city.xlsx
@@ -877,8 +877,8 @@
   </sheetPr>
   <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -904,7 +904,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -932,7 +932,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>23</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>23</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>23</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -1226,7 +1226,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>23</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>23</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>23</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>23</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>23</v>
@@ -1338,7 +1338,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>23</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>60</v>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>60</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>60</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>60</v>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>60</v>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>60</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>60</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>60</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>60</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>60</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>60</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>80</v>
@@ -1520,7 +1520,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>80</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>80</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>80</v>
@@ -1562,7 +1562,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>80</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>80</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>80</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>80</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>80</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>97</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>97</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>97</v>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>97</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>97</v>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>97</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>97</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>97</v>
@@ -1744,7 +1744,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>97</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>97</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>97</v>
@@ -1786,7 +1786,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>97</v>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>97</v>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>97</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>97</v>
@@ -1842,7 +1842,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>97</v>
@@ -1856,7 +1856,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>97</v>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>127</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>127</v>
@@ -1898,7 +1898,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>127</v>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>127</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>127</v>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>127</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>127</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>127</v>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>127</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>127</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>143</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>143</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>143</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>143</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>143</v>
@@ -2080,7 +2080,7 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>143</v>
@@ -2094,7 +2094,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>143</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>143</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>143</v>
@@ -2136,7 +2136,7 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>143</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>143</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>143</v>
@@ -2178,7 +2178,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>143</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>143</v>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>143</v>
@@ -2220,7 +2220,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>143</v>
@@ -2234,7 +2234,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>143</v>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>143</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>143</v>
@@ -2276,7 +2276,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>143</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>143</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>143</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>143</v>
@@ -2332,7 +2332,7 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>143</v>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>143</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>143</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>143</v>
@@ -2388,7 +2388,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>143</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>143</v>
@@ -2416,7 +2416,7 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>143</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>143</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>143</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>143</v>
@@ -2472,7 +2472,7 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>143</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>196</v>
@@ -2500,7 +2500,7 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>196</v>
@@ -2514,7 +2514,7 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>196</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>196</v>
@@ -2542,7 +2542,7 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>196</v>
@@ -2556,7 +2556,7 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>196</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>196</v>
@@ -2584,7 +2584,7 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>196</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>196</v>
@@ -2612,7 +2612,7 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>196</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>196</v>
@@ -2640,7 +2640,7 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>196</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>196</v>

</xml_diff>